<commit_message>
Update Burn down  + Test Plan
</commit_message>
<xml_diff>
--- a/Document/SprintBurnDown.xlsx
+++ b/Document/SprintBurnDown.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="24380" windowHeight="14680"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="24380" windowHeight="14680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 4" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -37,51 +37,6 @@
   </si>
   <si>
     <t>Time (left)</t>
-  </si>
-  <si>
-    <t>Team documentation</t>
-  </si>
-  <si>
-    <t>Wireframing</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>HTML/CSS</t>
-  </si>
-  <si>
-    <t>Theme development</t>
-  </si>
-  <si>
-    <t>Server setup</t>
-  </si>
-  <si>
-    <t>Testing 1</t>
-  </si>
-  <si>
-    <t>Bug fixes</t>
-  </si>
-  <si>
-    <t>Optimization</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>SEO</t>
-  </si>
-  <si>
-    <t>User documentation</t>
-  </si>
-  <si>
-    <t>Go live</t>
-  </si>
-  <si>
-    <t>Testing 2</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -151,6 +106,21 @@
   </si>
   <si>
     <t xml:space="preserve">DLT/PVC can view CMR </t>
+  </si>
+  <si>
+    <t>Create job to auto reject overdate report daily</t>
+  </si>
+  <si>
+    <t>DLT comment CMR</t>
+  </si>
+  <si>
+    <t>DLT/PVC can view CMR</t>
+  </si>
+  <si>
+    <t>View circle chart in CMR details page</t>
+  </si>
+  <si>
+    <t>Edit create CMR page</t>
   </si>
 </sst>
 </file>
@@ -583,7 +553,397 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE69999"/>
+          <bgColor rgb="FFE69999"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE69999"/>
+          <bgColor rgb="FFE69999"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF003366"/>
@@ -1181,11 +1541,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2109124848"/>
-        <c:axId val="-2076484560"/>
+        <c:axId val="2132289056"/>
+        <c:axId val="2137763376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109124848"/>
+        <c:axId val="2132289056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,7 +1584,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076484560"/>
+        <c:crossAx val="2137763376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1232,7 +1592,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076484560"/>
+        <c:axId val="2137763376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,7 +1636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2109124848"/>
+        <c:crossAx val="2132289056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1589,11 +1949,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2109021296"/>
-        <c:axId val="-2109016112"/>
+        <c:axId val="-2073637216"/>
+        <c:axId val="-2126598432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109021296"/>
+        <c:axId val="-2073637216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,6 +1975,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1631,7 +1992,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2109016112"/>
+        <c:crossAx val="-2126598432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1639,7 +2000,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109016112"/>
+        <c:axId val="-2126598432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1661,6 +2022,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1682,13 +2044,332 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2109021296"/>
+        <c:crossAx val="-2073637216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$C$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Burnout</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3D85C6"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 4'!$D$37:$AC$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>510.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>425.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>340.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>255.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$D$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>510.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>375.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>325.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>245.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Estimate</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$D$37:$J$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>510.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>425.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>340.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>255.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2136710400"/>
+        <c:axId val="2130897952"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2136710400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days in Calendar</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2130897952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2130897952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hours left</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2136710400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1767,6 +2448,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2040,11 +2753,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2325,7 +3038,7 @@
     </row>
     <row r="3" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6">
         <v>0</v>
@@ -2402,7 +3115,7 @@
     </row>
     <row r="4" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B4" s="14">
         <v>30</v>
@@ -2424,7 +3137,7 @@
     </row>
     <row r="5" spans="1:65" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B5" s="14">
         <v>30</v>
@@ -2448,7 +3161,7 @@
     </row>
     <row r="6" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B6" s="14">
         <v>10</v>
@@ -2467,7 +3180,7 @@
     </row>
     <row r="7" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B7" s="14">
         <v>50</v>
@@ -2487,7 +3200,7 @@
     </row>
     <row r="8" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B8" s="14">
         <v>130</v>
@@ -2513,7 +3226,7 @@
     </row>
     <row r="9" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B9" s="14">
         <v>20</v>
@@ -2539,7 +3252,7 @@
     </row>
     <row r="10" spans="1:65" ht="39" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B10" s="14">
         <v>10</v>
@@ -2561,7 +3274,7 @@
     </row>
     <row r="11" spans="1:65" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B11" s="14">
         <v>10</v>
@@ -2583,7 +3296,7 @@
     </row>
     <row r="12" spans="1:65" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B12" s="14">
         <v>80</v>
@@ -2609,7 +3322,7 @@
     </row>
     <row r="13" spans="1:65" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B13" s="14">
         <v>40</v>
@@ -2631,7 +3344,7 @@
     </row>
     <row r="14" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="13" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B14" s="14">
         <v>30</v>
@@ -2651,7 +3364,7 @@
     </row>
     <row r="15" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="13" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B15" s="14">
         <v>20</v>
@@ -2676,7 +3389,7 @@
     </row>
     <row r="16" spans="1:65" ht="26" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B16" s="14">
         <v>20</v>
@@ -2702,7 +3415,7 @@
     </row>
     <row r="17" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B17" s="14">
         <v>30</v>
@@ -3022,7 +3735,7 @@
     </row>
     <row r="35" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="25" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B35" s="26">
         <f t="shared" ref="B35:D35" si="2">SUM(B3:B34)</f>
@@ -3283,7 +3996,7 @@
     </row>
     <row r="36" spans="1:65" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" s="29" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B36" s="30">
         <f>B35-SUM(E36:BL36)</f>
@@ -3397,11 +4110,11 @@
     </row>
     <row r="37" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="37" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B37" s="38"/>
       <c r="C37" s="39" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D37" s="40">
         <f>B35</f>
@@ -3654,11 +4367,11 @@
     </row>
     <row r="38" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="37" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B38" s="38"/>
       <c r="C38" s="39" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D38" s="40">
         <f>C35</f>
@@ -3911,7 +4624,7 @@
     </row>
     <row r="39" spans="1:65" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="46" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B39" s="47"/>
       <c r="C39" s="47"/>
@@ -3979,7 +4692,7 @@
     </row>
     <row r="40" spans="1:65" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="48" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B40" s="47"/>
       <c r="C40" s="47"/>
@@ -4234,62 +4947,62 @@
     <mergeCell ref="A40:D40"/>
   </mergeCells>
   <conditionalFormatting sqref="A37:BM38">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:BM34">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4305,8 +5018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM101"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4586,30 +5299,24 @@
       <c r="BL2" s="3"/>
       <c r="BM2" s="3"/>
     </row>
-    <row r="3" spans="1:65" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:65" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="6">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" ref="C3:C34" si="0">IF(B3&lt;SUM(E3:BL3),SUM(E3:BL3),B3)</f>
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" ref="D3:D34" si="1">IF(C3&gt;B3,$C3-(SUM($E3:$BM3)),$B3-(SUM($E3:$BM3)))</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="9">
-        <v>4</v>
-      </c>
-      <c r="F3" s="11">
-        <v>1</v>
-      </c>
-      <c r="G3" s="11">
-        <v>1</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -4671,377 +5378,278 @@
     </row>
     <row r="4" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" s="19">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4" s="15"/>
-      <c r="F4" s="16">
-        <v>3</v>
-      </c>
-      <c r="G4" s="16">
-        <v>1</v>
-      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
       <c r="BM4" s="17"/>
     </row>
     <row r="5" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B5" s="19">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E5" s="15"/>
-      <c r="F5" s="16">
-        <v>8</v>
-      </c>
-      <c r="G5" s="16">
-        <v>2</v>
-      </c>
-      <c r="H5" s="16">
-        <v>1</v>
-      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="BM5" s="17"/>
     </row>
     <row r="6" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B6" s="19">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E6" s="15"/>
-      <c r="H6" s="16">
-        <v>3</v>
-      </c>
+      <c r="H6" s="16"/>
       <c r="BM6" s="17"/>
     </row>
-    <row r="7" spans="1:65" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:65" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B7" s="19">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="I7" s="16">
-        <v>4</v>
-      </c>
-      <c r="J7" s="16">
-        <v>4</v>
-      </c>
+      <c r="F7" s="45">
+        <v>80</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
       <c r="BM7" s="17"/>
     </row>
     <row r="8" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B8" s="19">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="K8" s="16">
-        <v>6</v>
-      </c>
-      <c r="L8" s="16">
-        <v>2</v>
-      </c>
+      <c r="E8" s="15">
+        <v>30</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
       <c r="BM8" s="17"/>
     </row>
     <row r="9" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B9" s="19">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="L9" s="16">
-        <v>4</v>
-      </c>
-      <c r="M9" s="16">
-        <v>8</v>
-      </c>
+      <c r="E9" s="15">
+        <v>30</v>
+      </c>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
       <c r="BM9" s="17"/>
     </row>
     <row r="10" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="19">
-        <v>4</v>
-      </c>
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="1"/>
+        <f>IF(C10&gt;B10,$C10-(SUM($E10:$BM10)),$B10-(SUM($E10:$BM10)))</f>
         <v>0</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="N10" s="16">
-        <v>2</v>
-      </c>
-      <c r="O10" s="16">
-        <v>2</v>
-      </c>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
       <c r="BM10" s="17"/>
     </row>
     <row r="11" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="19">
-        <v>3</v>
-      </c>
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E11" s="15"/>
-      <c r="O11" s="16">
-        <v>2</v>
-      </c>
-      <c r="P11" s="16">
-        <v>1</v>
-      </c>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
       <c r="BM11" s="17"/>
     </row>
     <row r="12" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="19">
-        <v>4</v>
-      </c>
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="P12" s="16">
-        <v>4</v>
-      </c>
-      <c r="Q12" s="16">
-        <v>1</v>
-      </c>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
       <c r="BM12" s="17"/>
     </row>
     <row r="13" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="19">
-        <v>4</v>
-      </c>
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E13" s="15"/>
-      <c r="Q13" s="16">
-        <v>4</v>
-      </c>
+      <c r="Q13" s="16"/>
       <c r="BM13" s="17"/>
     </row>
     <row r="14" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="19">
-        <v>5</v>
-      </c>
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E14" s="15"/>
-      <c r="R14" s="16">
-        <v>3</v>
-      </c>
-      <c r="S14" s="16">
-        <v>3</v>
-      </c>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
       <c r="BM14" s="17"/>
     </row>
     <row r="15" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="19">
-        <v>10</v>
-      </c>
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="7">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D15" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="R15" s="16">
-        <v>2</v>
-      </c>
-      <c r="S15" s="16">
-        <v>1</v>
-      </c>
-      <c r="T15" s="16">
-        <v>4</v>
-      </c>
-      <c r="U15" s="16">
-        <v>3</v>
-      </c>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
       <c r="BM15" s="17"/>
     </row>
     <row r="16" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="19">
-        <v>8</v>
-      </c>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D16" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E16" s="15"/>
-      <c r="R16" s="16">
-        <v>1</v>
-      </c>
-      <c r="U16" s="16">
-        <v>2</v>
-      </c>
-      <c r="V16" s="16">
-        <v>3</v>
-      </c>
-      <c r="W16" s="16">
-        <v>1</v>
-      </c>
-      <c r="X16" s="16">
-        <v>1</v>
-      </c>
+      <c r="R16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
       <c r="BM16" s="17"/>
     </row>
     <row r="17" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="19">
-        <v>2</v>
-      </c>
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E17" s="15"/>
-      <c r="V17" s="16">
-        <v>1</v>
-      </c>
-      <c r="W17" s="16">
-        <v>1</v>
-      </c>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
       <c r="BM17" s="17"/>
     </row>
     <row r="18" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="19">
-        <v>5</v>
-      </c>
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E18" s="15"/>
-      <c r="V18" s="16">
-        <v>1</v>
-      </c>
-      <c r="W18" s="16">
-        <v>1</v>
-      </c>
-      <c r="X18" s="16">
-        <v>3</v>
-      </c>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
       <c r="BM18" s="17"/>
     </row>
     <row r="19" spans="1:65" ht="13" x14ac:dyDescent="0.15">
@@ -5329,99 +5937,99 @@
     </row>
     <row r="35" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="25" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B35" s="26">
         <f t="shared" ref="B35:D35" si="2">SUM(B3:B34)</f>
-        <v>88</v>
+        <v>320</v>
       </c>
       <c r="C35" s="27">
         <f t="shared" si="2"/>
-        <v>99</v>
+        <v>320</v>
       </c>
       <c r="D35" s="27">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E35" s="28">
         <f t="shared" ref="E35:BM35" si="3">SUM(E3:E19)</f>
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="F35" s="28">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="G35" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H35" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I35" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J35" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K35" s="28">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L35" s="28">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M35" s="28">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N35" s="28">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O35" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P35" s="28">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="28">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R35" s="28">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S35" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T35" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U35" s="28">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V35" s="28">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W35" s="28">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X35" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y35" s="28">
         <f t="shared" si="3"/>
@@ -5590,7 +6198,7 @@
     </row>
     <row r="36" spans="1:65" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" s="29" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B36" s="30">
         <f>B35-SUM(E36:BL36)</f>
@@ -5599,64 +6207,64 @@
       <c r="C36" s="31"/>
       <c r="D36" s="32"/>
       <c r="E36" s="33">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="F36" s="35">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="G36" s="35">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="H36" s="35">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="I36" s="35">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J36" s="35">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="K36" s="35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M36" s="35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P36" s="35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T36" s="35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W36" s="35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="X36" s="35">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y36" s="35">
         <v>0</v>
@@ -5704,91 +6312,91 @@
     </row>
     <row r="37" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="37" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B37" s="40"/>
       <c r="C37" s="39" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D37" s="40">
         <f>B35</f>
-        <v>88</v>
+        <v>320</v>
       </c>
       <c r="E37" s="42">
         <f t="shared" ref="E37:BM37" si="4">D37-E36</f>
-        <v>83</v>
+        <v>266</v>
       </c>
       <c r="F37" s="42">
         <f t="shared" si="4"/>
-        <v>79</v>
+        <v>213</v>
       </c>
       <c r="G37" s="42">
         <f t="shared" si="4"/>
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="H37" s="42">
         <f t="shared" si="4"/>
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="I37" s="42">
         <f t="shared" si="4"/>
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="J37" s="42">
         <f t="shared" si="4"/>
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="K37" s="42">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="L37" s="42">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="M37" s="42">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="N37" s="42">
         <f t="shared" si="4"/>
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="O37" s="42">
         <f t="shared" si="4"/>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="P37" s="42">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="42">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R37" s="42">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="S37" s="42">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="T37" s="42">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="U37" s="42">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="V37" s="42">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="W37" s="42">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X37" s="42">
         <f t="shared" si="4"/>
@@ -5961,264 +6569,264 @@
     </row>
     <row r="38" spans="1:65" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="37" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B38" s="40"/>
       <c r="C38" s="39" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D38" s="40">
         <f>C35</f>
-        <v>99</v>
+        <v>320</v>
       </c>
       <c r="E38" s="40">
         <f>$C$35-SUM(E$3:E$34)</f>
-        <v>95</v>
+        <v>260</v>
       </c>
       <c r="F38" s="40">
         <f t="shared" ref="F38:BM38" si="5">E38-SUM(F3:F34)</f>
-        <v>83</v>
+        <v>180</v>
       </c>
       <c r="G38" s="40">
         <f t="shared" si="5"/>
-        <v>79</v>
+        <v>180</v>
       </c>
       <c r="H38" s="40">
         <f t="shared" si="5"/>
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="I38" s="40">
         <f t="shared" si="5"/>
-        <v>71</v>
+        <v>180</v>
       </c>
       <c r="J38" s="40">
         <f t="shared" si="5"/>
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="K38" s="40">
         <f t="shared" si="5"/>
-        <v>61</v>
+        <v>180</v>
       </c>
       <c r="L38" s="40">
         <f t="shared" si="5"/>
-        <v>55</v>
+        <v>180</v>
       </c>
       <c r="M38" s="40">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>180</v>
       </c>
       <c r="N38" s="40">
         <f t="shared" si="5"/>
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="O38" s="40">
         <f t="shared" si="5"/>
-        <v>41</v>
+        <v>180</v>
       </c>
       <c r="P38" s="40">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>180</v>
       </c>
       <c r="Q38" s="40">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>180</v>
       </c>
       <c r="R38" s="40">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="S38" s="40">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="T38" s="40">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>180</v>
       </c>
       <c r="U38" s="40">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="V38" s="40">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>180</v>
       </c>
       <c r="W38" s="40">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>180</v>
       </c>
       <c r="X38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="Y38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="Z38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AA38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AB38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AC38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AD38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AE38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AF38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AG38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AH38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AI38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AJ38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AK38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AL38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AM38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AN38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AO38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AP38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AQ38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AR38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AS38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AT38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AU38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AV38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AW38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AX38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AY38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AZ38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BA38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BB38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BC38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BD38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BE38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BF38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BG38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BH38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BI38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BJ38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BK38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BL38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="BM38" s="40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:65" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="46" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B39" s="47"/>
       <c r="C39" s="47"/>
@@ -6286,7 +6894,7 @@
     </row>
     <row r="40" spans="1:65" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="48" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B40" s="47"/>
       <c r="C40" s="47"/>
@@ -6541,62 +7149,62 @@
     <mergeCell ref="A40:D40"/>
   </mergeCells>
   <conditionalFormatting sqref="A37:BM38">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:BM34">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update burn down and test plan
</commit_message>
<xml_diff>
--- a/Document/SprintBurnDown.xlsx
+++ b/Document/SprintBurnDown.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -121,6 +121,27 @@
   </si>
   <si>
     <t>Edit create CMR page</t>
+  </si>
+  <si>
+    <t>View number of Active/Pending/Reported in course list</t>
+  </si>
+  <si>
+    <t>Course can be cancel</t>
+  </si>
+  <si>
+    <t>Commit latest code of Linh</t>
+  </si>
+  <si>
+    <t>Edit display of table without records</t>
+  </si>
+  <si>
+    <t>Edit Logic of Delete Users</t>
+  </si>
+  <si>
+    <t>Table is not responsive</t>
+  </si>
+  <si>
+    <t>Insert 2 users of 2 role DLT &amp; PVC</t>
   </si>
 </sst>
 </file>
@@ -553,397 +574,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <font>
-        <color rgb="FF003366"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF003366"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE69999"/>
-          <bgColor rgb="FFE69999"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE69999"/>
-          <bgColor rgb="FFE69999"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFADCB3"/>
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF6600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFADCB3"/>
-          <bgColor rgb="FFFADCB3"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFCC00"/>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFCC00"/>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="1"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF003366"/>
@@ -1541,11 +1172,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2132289056"/>
-        <c:axId val="2137763376"/>
+        <c:axId val="-2107263744"/>
+        <c:axId val="2103342032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132289056"/>
+        <c:axId val="-2107263744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,7 +1215,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137763376"/>
+        <c:crossAx val="2103342032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1592,7 +1223,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137763376"/>
+        <c:axId val="2103342032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1267,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132289056"/>
+        <c:crossAx val="-2107263744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1949,11 +1580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2073637216"/>
-        <c:axId val="-2126598432"/>
+        <c:axId val="2143404736"/>
+        <c:axId val="-2108513712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2073637216"/>
+        <c:axId val="2143404736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1992,7 +1623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126598432"/>
+        <c:crossAx val="-2108513712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2000,7 +1631,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126598432"/>
+        <c:axId val="-2108513712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2044,7 +1675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2073637216"/>
+        <c:crossAx val="2143404736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2091,7 +1722,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 4'!$C$38</c:f>
+              <c:f>'Sprint 5'!$C$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2187,30 +1818,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$D$38:$J$38</c:f>
+              <c:f>'Sprint 5'!$D$38:$J$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>510.0</c:v>
+                  <c:v>415.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>490.0</c:v>
+                  <c:v>355.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>375.0</c:v>
+                  <c:v>275.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>325.0</c:v>
+                  <c:v>185.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>245.0</c:v>
+                  <c:v>185.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>160.0</c:v>
+                  <c:v>185.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120.0</c:v>
+                  <c:v>185.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,27 +1859,27 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$D$37:$J$37</c:f>
+              <c:f>'Sprint 5'!$D$37:$J$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>510.0</c:v>
+                  <c:v>415.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>425.0</c:v>
+                  <c:v>346.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>340.0</c:v>
+                  <c:v>276.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>255.0</c:v>
+                  <c:v>207.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>170.0</c:v>
+                  <c:v>138.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>85.0</c:v>
+                  <c:v>69.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -2267,11 +1898,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2136710400"/>
-        <c:axId val="2130897952"/>
+        <c:axId val="2103789040"/>
+        <c:axId val="2103794224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2136710400"/>
+        <c:axId val="2103789040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2310,7 +1941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130897952"/>
+        <c:crossAx val="2103794224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2318,7 +1949,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130897952"/>
+        <c:axId val="2103794224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2362,7 +1993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136710400"/>
+        <c:crossAx val="2103789040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2754,7 +2385,7 @@
   <dimension ref="A1:BM101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" sqref="A1:XFD1048576"/>
@@ -4947,62 +4578,62 @@
     <mergeCell ref="A40:D40"/>
   </mergeCells>
   <conditionalFormatting sqref="A37:BM38">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:BM34">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="41" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="40" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="38" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="36" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5018,8 +4649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5389,11 +5020,13 @@
       </c>
       <c r="D4" s="8">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16">
+        <v>10</v>
+      </c>
       <c r="BM4" s="17"/>
     </row>
     <row r="5" spans="1:65" ht="13" x14ac:dyDescent="0.15">
@@ -5409,11 +5042,13 @@
       </c>
       <c r="D5" s="8">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="G5" s="16">
+        <v>50</v>
+      </c>
       <c r="H5" s="16"/>
       <c r="BM5" s="17"/>
     </row>
@@ -5503,16 +5138,20 @@
       <c r="M9" s="16"/>
       <c r="BM9" s="17"/>
     </row>
-    <row r="10" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
+    <row r="10" spans="1:65" ht="26" x14ac:dyDescent="0.15">
+      <c r="A10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="19">
+        <v>10</v>
+      </c>
       <c r="C10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D10" s="8">
         <f>IF(C10&gt;B10,$C10-(SUM($E10:$BM10)),$B10-(SUM($E10:$BM10)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E10" s="15"/>
       <c r="N10" s="16"/>
@@ -5520,15 +5159,19 @@
       <c r="BM10" s="17"/>
     </row>
     <row r="11" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="19">
+        <v>20</v>
+      </c>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E11" s="15"/>
       <c r="O11" s="16"/>
@@ -5536,64 +5179,83 @@
       <c r="BM11" s="17"/>
     </row>
     <row r="12" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="19">
+        <v>10</v>
+      </c>
       <c r="C12" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E12" s="15"/>
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="BM12" s="17"/>
     </row>
-    <row r="13" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
+    <row r="13" spans="1:65" ht="26" x14ac:dyDescent="0.15">
+      <c r="A13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="19">
+        <v>10</v>
+      </c>
       <c r="C13" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D13" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E13" s="15"/>
       <c r="Q13" s="16"/>
       <c r="BM13" s="17"/>
     </row>
     <row r="14" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="19">
+        <v>15</v>
+      </c>
       <c r="C14" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E14" s="15"/>
       <c r="R14" s="16"/>
       <c r="S14" s="16"/>
       <c r="BM14" s="17"/>
     </row>
-    <row r="15" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
+    <row r="15" spans="1:65" ht="39" x14ac:dyDescent="0.15">
+      <c r="A15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="19">
+        <v>10</v>
+      </c>
       <c r="C15" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D15" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E15" s="15"/>
+      <c r="G15" s="45">
+        <v>10</v>
+      </c>
       <c r="R15" s="16"/>
       <c r="S15" s="16"/>
       <c r="T15" s="16"/>
@@ -5601,17 +5263,24 @@
       <c r="BM15" s="17"/>
     </row>
     <row r="16" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="19">
+        <v>20</v>
+      </c>
       <c r="C16" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D16" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E16" s="15"/>
+      <c r="G16" s="45">
+        <v>20</v>
+      </c>
       <c r="R16" s="16"/>
       <c r="U16" s="16"/>
       <c r="V16" s="16"/>
@@ -5941,15 +5610,15 @@
       </c>
       <c r="B35" s="26">
         <f t="shared" ref="B35:D35" si="2">SUM(B3:B34)</f>
-        <v>320</v>
+        <v>415</v>
       </c>
       <c r="C35" s="27">
         <f t="shared" si="2"/>
-        <v>320</v>
+        <v>415</v>
       </c>
       <c r="D35" s="27">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E35" s="28">
         <f t="shared" ref="E35:BM35" si="3">SUM(E3:E19)</f>
@@ -5961,7 +5630,7 @@
       </c>
       <c r="G35" s="28">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H35" s="28">
         <f t="shared" si="3"/>
@@ -6207,22 +5876,22 @@
       <c r="C36" s="31"/>
       <c r="D36" s="32"/>
       <c r="E36" s="33">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="F36" s="35">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="G36" s="35">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="H36" s="35">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="I36" s="35">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="J36" s="35">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="K36" s="35">
         <v>0</v>
@@ -6320,27 +5989,27 @@
       </c>
       <c r="D37" s="40">
         <f>B35</f>
-        <v>320</v>
+        <v>415</v>
       </c>
       <c r="E37" s="42">
         <f t="shared" ref="E37:BM37" si="4">D37-E36</f>
-        <v>266</v>
+        <v>346</v>
       </c>
       <c r="F37" s="42">
         <f t="shared" si="4"/>
-        <v>213</v>
+        <v>276</v>
       </c>
       <c r="G37" s="42">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="H37" s="42">
         <f t="shared" si="4"/>
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="I37" s="42">
         <f t="shared" si="4"/>
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="J37" s="42">
         <f t="shared" si="4"/>
@@ -6577,251 +6246,251 @@
       </c>
       <c r="D38" s="40">
         <f>C35</f>
-        <v>320</v>
+        <v>415</v>
       </c>
       <c r="E38" s="40">
         <f>$C$35-SUM(E$3:E$34)</f>
-        <v>260</v>
+        <v>355</v>
       </c>
       <c r="F38" s="40">
         <f t="shared" ref="F38:BM38" si="5">E38-SUM(F3:F34)</f>
-        <v>180</v>
+        <v>275</v>
       </c>
       <c r="G38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="H38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="I38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="J38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="K38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="L38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="M38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="N38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="O38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="Q38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="R38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="S38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="T38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="U38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="V38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="W38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="X38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="Y38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="Z38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AA38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AB38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AC38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AD38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AE38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AF38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AG38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AH38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AI38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AJ38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AK38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AL38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AM38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AN38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AO38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AP38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AQ38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AR38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AS38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AT38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AU38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AV38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AW38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AX38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AY38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AZ38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BA38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BB38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BC38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BD38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BE38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BF38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BG38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BH38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BI38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BJ38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BK38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BL38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="BM38" s="40">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:65" ht="18" x14ac:dyDescent="0.2">
@@ -7149,62 +6818,62 @@
     <mergeCell ref="A40:D40"/>
   </mergeCells>
   <conditionalFormatting sqref="A37:BM38">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:BM34">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D34">
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update Sprint Burndown and Test Plan
</commit_message>
<xml_diff>
--- a/Document/SprintBurnDown.xlsx
+++ b/Document/SprintBurnDown.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -160,7 +160,10 @@
     <t>Create summarize report</t>
   </si>
   <si>
-    <t>Write group report</t>
+    <t>Add char counter for comment</t>
+  </si>
+  <si>
+    <t>Add some Security Method to project</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -575,6 +578,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1389,11 +1395,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2128105184"/>
-        <c:axId val="-2064024944"/>
+        <c:axId val="-2070394416"/>
+        <c:axId val="2125624080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2128105184"/>
+        <c:axId val="-2070394416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,7 +1437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064024944"/>
+        <c:crossAx val="2125624080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1439,7 +1445,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2064024944"/>
+        <c:axId val="2125624080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1488,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128105184"/>
+        <c:crossAx val="-2070394416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1794,11 +1800,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2103911568"/>
-        <c:axId val="2101235440"/>
+        <c:axId val="-2098633584"/>
+        <c:axId val="-2098628400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103911568"/>
+        <c:axId val="-2098633584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1826,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1837,7 +1842,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101235440"/>
+        <c:crossAx val="-2098628400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1845,7 +1850,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101235440"/>
+        <c:axId val="-2098628400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +1872,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1889,14 +1893,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103911568"/>
+        <c:crossAx val="-2098633584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2112,11 +2115,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2064631600"/>
-        <c:axId val="-2066932928"/>
+        <c:axId val="-2098616208"/>
+        <c:axId val="-2098611024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2064631600"/>
+        <c:axId val="-2098616208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2138,7 +2141,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2155,7 +2157,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066932928"/>
+        <c:crossAx val="-2098611024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2163,7 +2165,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2066932928"/>
+        <c:axId val="-2098611024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2185,7 +2187,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2207,14 +2208,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064631600"/>
+        <c:crossAx val="-2098616208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2520,11 +2520,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2064593552"/>
-        <c:axId val="-2066545984"/>
+        <c:axId val="-2098526144"/>
+        <c:axId val="-2098520960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2064593552"/>
+        <c:axId val="-2098526144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2563,7 +2563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066545984"/>
+        <c:crossAx val="-2098520960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2571,7 +2571,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2066545984"/>
+        <c:axId val="-2098520960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2615,7 +2615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064593552"/>
+        <c:crossAx val="-2098526144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2763,25 +2763,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>530.0</c:v>
+                  <c:v>380.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>280.0</c:v>
+                  <c:v>130.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>110.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300.0</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>300.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>300.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2804,22 +2804,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>530.0</c:v>
+                  <c:v>420.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>442.0</c:v>
+                  <c:v>350.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>353.0</c:v>
+                  <c:v>280.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265.0</c:v>
+                  <c:v>210.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>177.0</c:v>
+                  <c:v>140.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88.0</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -2838,11 +2838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2063661936"/>
-        <c:axId val="-2098736816"/>
+        <c:axId val="-2098488192"/>
+        <c:axId val="-2098483008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2063661936"/>
+        <c:axId val="-2098488192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2881,7 +2881,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098736816"/>
+        <c:crossAx val="-2098483008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2889,7 +2889,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098736816"/>
+        <c:axId val="-2098483008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2933,7 +2933,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063661936"/>
+        <c:crossAx val="-2098488192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5263,12 +5263,12 @@
       </c>
     </row>
     <row r="39" spans="1:65" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
       <c r="F39" s="43"/>
       <c r="G39" s="43"/>
       <c r="H39" s="43"/>
@@ -5331,12 +5331,12 @@
       <c r="BM39" s="43"/>
     </row>
     <row r="40" spans="1:65" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
       <c r="H40" s="43"/>
@@ -7517,12 +7517,12 @@
       </c>
     </row>
     <row r="39" spans="1:65" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
       <c r="F39" s="43"/>
       <c r="G39" s="43"/>
       <c r="H39" s="43"/>
@@ -7585,12 +7585,12 @@
       <c r="BM39" s="43"/>
     </row>
     <row r="40" spans="1:65" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
       <c r="H40" s="43"/>
@@ -7912,8 +7912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8351,9 +8351,12 @@
       </c>
       <c r="D7" s="8">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="46">
         <v>10</v>
       </c>
-      <c r="E7" s="15"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="BM7" s="17"/>
@@ -8371,9 +8374,12 @@
       </c>
       <c r="D8" s="8">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="H8" s="46">
         <v>40</v>
       </c>
-      <c r="E8" s="15"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
       <c r="BM8" s="17"/>
@@ -8383,57 +8389,65 @@
         <v>43</v>
       </c>
       <c r="B9" s="19">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="C9" s="7">
         <v>200</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E9" s="15">
         <v>170</v>
-      </c>
-      <c r="F9" s="46">
-        <v>-20</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="BM9" s="17"/>
     </row>
-    <row r="10" spans="1:65" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:65" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="19">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="D10" s="8">
         <f>IF(C10&gt;B10,$C10-(SUM($E10:$BM10)),$B10-(SUM($E10:$BM10)))</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E10" s="15"/>
+      <c r="G10" s="46">
+        <v>40</v>
+      </c>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="BM10" s="17"/>
     </row>
     <row r="11" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="19">
+        <v>10</v>
+      </c>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E11" s="15"/>
+      <c r="F11" s="46">
+        <v>10</v>
+      </c>
+      <c r="G11" s="47"/>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
       <c r="BM11" s="17"/>
@@ -8844,15 +8858,15 @@
       </c>
       <c r="B35" s="26">
         <f t="shared" ref="B35:D35" si="2">SUM(B3:B34)</f>
-        <v>530</v>
+        <v>420</v>
       </c>
       <c r="C35" s="27">
         <f t="shared" si="2"/>
-        <v>530</v>
+        <v>380</v>
       </c>
       <c r="D35" s="27">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>70</v>
       </c>
       <c r="E35" s="28">
         <f t="shared" ref="E35:BM35" si="3">SUM(E3:E19)</f>
@@ -8860,15 +8874,15 @@
       </c>
       <c r="F35" s="28">
         <f t="shared" si="3"/>
-        <v>-20</v>
+        <v>20</v>
       </c>
       <c r="G35" s="28">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H35" s="28">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I35" s="28">
         <f t="shared" si="3"/>
@@ -9110,22 +9124,22 @@
       <c r="C36" s="31"/>
       <c r="D36" s="32"/>
       <c r="E36" s="33">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F36" s="35">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="G36" s="35">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="H36" s="35">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="I36" s="35">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="J36" s="35">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="K36" s="35">
         <v>0</v>
@@ -9223,27 +9237,27 @@
       </c>
       <c r="D37" s="40">
         <f>B35</f>
-        <v>530</v>
+        <v>420</v>
       </c>
       <c r="E37" s="42">
         <f t="shared" ref="E37:BM37" si="4">D37-E36</f>
-        <v>442</v>
+        <v>350</v>
       </c>
       <c r="F37" s="42">
         <f t="shared" si="4"/>
-        <v>353</v>
+        <v>280</v>
       </c>
       <c r="G37" s="42">
         <f t="shared" si="4"/>
-        <v>265</v>
+        <v>210</v>
       </c>
       <c r="H37" s="42">
         <f t="shared" si="4"/>
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="I37" s="42">
         <f t="shared" si="4"/>
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="J37" s="42">
         <f t="shared" si="4"/>
@@ -9480,260 +9494,260 @@
       </c>
       <c r="D38" s="40">
         <f>C35</f>
-        <v>530</v>
+        <v>380</v>
       </c>
       <c r="E38" s="40">
         <f>$C$35-SUM(E$3:E$34)</f>
-        <v>280</v>
+        <v>130</v>
       </c>
       <c r="F38" s="40">
         <f t="shared" ref="F38:BM38" si="5">E38-SUM(F3:F34)</f>
-        <v>300</v>
+        <v>110</v>
       </c>
       <c r="G38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>70</v>
       </c>
       <c r="H38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="I38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="J38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="K38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="L38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="M38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="N38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="O38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="P38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="Q38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="R38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="S38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="T38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="U38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="V38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="W38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="X38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="Y38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="Z38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AA38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AB38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AC38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AD38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AE38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AF38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AG38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AH38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AI38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AJ38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AK38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AL38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AM38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AN38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AO38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AP38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AQ38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AR38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AS38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AT38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AU38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AV38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AW38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AX38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AY38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="AZ38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BA38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BB38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BC38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BD38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BE38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BF38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BG38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BH38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BI38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BJ38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BK38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BL38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="BM38" s="40">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:65" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
       <c r="F39" s="43"/>
       <c r="G39" s="43"/>
       <c r="H39" s="43"/>
@@ -9796,12 +9810,12 @@
       <c r="BM39" s="43"/>
     </row>
     <row r="40" spans="1:65" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
       <c r="H40" s="43"/>

</xml_diff>